<commit_message>
printing page small bug fixed
</commit_message>
<xml_diff>
--- a/config/reconstruct/ti-le-choi.xlsx
+++ b/config/reconstruct/ti-le-choi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\search_project\config\reconstruct\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305E49A2-ABA4-49D7-BC0D-92C52D162C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3972D-3135-48A4-89ED-1E91497486C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="21600" windowHeight="10650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="10650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1286,15 +1286,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V108" sqref="V108"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="14" width="9.140625" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="14" width="9.140625" customWidth="1"/>
     <col min="15" max="15" width="8.7109375" customWidth="1"/>
     <col min="16" max="18" width="9.140625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
add data of 2022, bug fixed in printing page
</commit_message>
<xml_diff>
--- a/config/reconstruct/ti-le-choi.xlsx
+++ b/config/reconstruct/ti-le-choi.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\search_project\config\reconstruct\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Long To\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F3972D-3135-48A4-89ED-1E91497486C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51D2AC61-112A-469D-9EBE-F1198D0EC8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="0" windowWidth="21600" windowHeight="10650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="134">
   <si>
     <t>STT</t>
   </si>
@@ -385,6 +395,9 @@
 Huyện</t>
   </si>
   <si>
+    <t>B.Thạnh</t>
+  </si>
+  <si>
     <t>Gò Vấp</t>
   </si>
   <si>
@@ -425,43 +438,7 @@
 vọng</t>
   </si>
   <si>
-    <t>Quận 1</t>
-  </si>
-  <si>
-    <t>Quận 2</t>
-  </si>
-  <si>
-    <t>Quận 3</t>
-  </si>
-  <si>
-    <t>Quận 4</t>
-  </si>
-  <si>
-    <t>Quận 5</t>
-  </si>
-  <si>
-    <t>Quận 6</t>
-  </si>
-  <si>
-    <t>Quận 7</t>
-  </si>
-  <si>
-    <t>Quận 8</t>
-  </si>
-  <si>
-    <t>Quận 9</t>
-  </si>
-  <si>
-    <t>Quận 10</t>
-  </si>
-  <si>
-    <t>Quận 11</t>
-  </si>
-  <si>
-    <t>Quận 12</t>
-  </si>
-  <si>
-    <t>Bình Thạnh</t>
+    <t>Năm 2022-2023</t>
   </si>
 </sst>
 </file>
@@ -531,7 +508,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -553,12 +530,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -888,6 +859,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -921,6 +895,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -928,18 +908,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -957,15 +925,53 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEAAF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF49494"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1284,148 +1290,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X110"/>
+  <dimension ref="A1:AB110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AF11" sqref="AF11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" customWidth="1"/>
-    <col min="9" max="14" width="9.140625" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="18" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" hidden="1" customWidth="1"/>
+    <col min="4" max="14" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" hidden="1" customWidth="1"/>
+    <col min="16" max="18" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="19" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="23" max="24" width="7.85546875" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:27" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="32" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="32" t="s">
+      <c r="H1" s="36"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="K1" s="33"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="32" t="s">
+      <c r="K1" s="36"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="34"/>
-      <c r="P1" s="32" t="s">
+      <c r="N1" s="36"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="34"/>
-      <c r="S1" s="32" t="s">
+      <c r="Q1" s="36"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="T1" s="33"/>
-      <c r="U1" s="34"/>
-      <c r="V1" s="32" t="s">
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="W1" s="33"/>
-      <c r="X1" s="34"/>
-    </row>
-    <row r="2" spans="1:24" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="21" t="s">
+      <c r="W1" s="36"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="35" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="37"/>
+    </row>
+    <row r="2" spans="1:27" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="23" t="s">
+      <c r="E2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="F2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="I2" s="23" t="s">
+      <c r="H2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="I2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="L2" s="23" t="s">
+      <c r="K2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="L2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="O2" s="23" t="s">
+      <c r="N2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="21" t="s">
+      <c r="O2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="P2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="Q2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="R2" s="23" t="s">
+      <c r="Q2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="R2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="S2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="T2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="U2" s="23" t="s">
+      <c r="T2" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="U2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="V2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="X2" s="23" t="s">
+      <c r="W2" s="23" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X2" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y2" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA2" s="24" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="20" t="s">
-        <v>132</v>
+      <c r="C3" s="20">
+        <v>1</v>
       </c>
       <c r="D3" s="6">
         <v>2.13</v>
@@ -1475,10 +1493,10 @@
       <c r="S3" s="6">
         <v>2.13</v>
       </c>
-      <c r="T3" s="24">
-        <v>675</v>
-      </c>
-      <c r="U3" s="25">
+      <c r="T3" s="25">
+        <v>675</v>
+      </c>
+      <c r="U3" s="26">
         <v>1436</v>
       </c>
       <c r="V3" s="6">
@@ -1490,16 +1508,26 @@
       <c r="X3" s="7">
         <v>1349</v>
       </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y3" s="6">
+        <f>ROUND(AA3/Z3,2)</f>
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="Z3" s="2">
+        <v>675</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>132</v>
+      <c r="C4" s="20">
+        <v>1</v>
       </c>
       <c r="D4" s="6">
         <v>2.2400000000000002</v>
@@ -1549,10 +1577,10 @@
       <c r="S4" s="6">
         <v>2.02</v>
       </c>
-      <c r="T4" s="24">
+      <c r="T4" s="25">
         <v>585</v>
       </c>
-      <c r="U4" s="25">
+      <c r="U4" s="26">
         <v>1180</v>
       </c>
       <c r="V4" s="6">
@@ -1564,16 +1592,26 @@
       <c r="X4" s="7">
         <v>1219</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y4" s="6">
+        <f t="shared" ref="Y4:Y67" si="0">ROUND(AA4/Z4,2)</f>
+        <v>2.02</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>675</v>
+      </c>
+      <c r="AA4" s="7">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="20" t="s">
-        <v>132</v>
+      <c r="C5" s="20">
+        <v>1</v>
       </c>
       <c r="D5" s="6">
         <v>1.24</v>
@@ -1623,10 +1661,10 @@
       <c r="S5" s="6">
         <v>1.4</v>
       </c>
-      <c r="T5" s="24">
+      <c r="T5" s="25">
         <v>540</v>
       </c>
-      <c r="U5" s="25">
+      <c r="U5" s="26">
         <v>755</v>
       </c>
       <c r="V5" s="6">
@@ -1638,16 +1676,26 @@
       <c r="X5" s="7">
         <v>762</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y5" s="6">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>540</v>
+      </c>
+      <c r="AA5" s="7">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="20" t="s">
-        <v>132</v>
+      <c r="C6" s="20">
+        <v>1</v>
       </c>
       <c r="D6" s="8">
         <v>1.89</v>
@@ -1697,10 +1745,10 @@
       <c r="S6" s="8">
         <v>0.46</v>
       </c>
-      <c r="T6" s="24">
+      <c r="T6" s="25">
         <v>180</v>
       </c>
-      <c r="U6" s="25">
+      <c r="U6" s="26">
         <v>82</v>
       </c>
       <c r="V6" s="8">
@@ -1712,16 +1760,26 @@
       <c r="X6" s="9">
         <v>56</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>210</v>
+      </c>
+      <c r="AA6" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="20" t="s">
-        <v>132</v>
+      <c r="C7" s="20">
+        <v>1</v>
       </c>
       <c r="D7" s="8">
         <v>1.86</v>
@@ -1771,10 +1829,10 @@
       <c r="S7" s="8">
         <v>2.17</v>
       </c>
-      <c r="T7" s="24">
+      <c r="T7" s="25">
         <v>270</v>
       </c>
-      <c r="U7" s="25">
+      <c r="U7" s="26">
         <v>587</v>
       </c>
       <c r="V7" s="8">
@@ -1786,16 +1844,26 @@
       <c r="X7" s="9">
         <v>527</v>
       </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y7" s="6">
+        <f t="shared" si="0"/>
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>235</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>133</v>
+      <c r="C8" s="21">
+        <v>2</v>
       </c>
       <c r="D8" s="8">
         <v>1.1399999999999999</v>
@@ -1845,10 +1913,10 @@
       <c r="S8" s="8">
         <v>1.54</v>
       </c>
-      <c r="T8" s="24">
+      <c r="T8" s="25">
         <v>450</v>
       </c>
-      <c r="U8" s="25">
+      <c r="U8" s="26">
         <v>692</v>
       </c>
       <c r="V8" s="8">
@@ -1860,16 +1928,26 @@
       <c r="X8" s="9">
         <v>693</v>
       </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y8" s="6">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>450</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>133</v>
+      <c r="C9" s="21">
+        <v>2</v>
       </c>
       <c r="D9" s="8">
         <v>1.08</v>
@@ -1919,10 +1997,10 @@
       <c r="S9" s="8">
         <v>0.59</v>
       </c>
-      <c r="T9" s="24">
+      <c r="T9" s="25">
         <v>540</v>
       </c>
-      <c r="U9" s="25">
+      <c r="U9" s="26">
         <v>316</v>
       </c>
       <c r="V9" s="8">
@@ -1934,16 +2012,26 @@
       <c r="X9" s="9">
         <v>422</v>
       </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.63</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>630</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>134</v>
+      <c r="C10" s="21">
+        <v>3</v>
       </c>
       <c r="D10" s="8">
         <v>2.04</v>
@@ -1993,10 +2081,10 @@
       <c r="S10" s="8">
         <v>2.12</v>
       </c>
-      <c r="T10" s="24">
+      <c r="T10" s="25">
         <v>450</v>
       </c>
-      <c r="U10" s="25">
+      <c r="U10" s="26">
         <v>952</v>
       </c>
       <c r="V10" s="8">
@@ -2008,16 +2096,26 @@
       <c r="X10" s="9">
         <v>1041</v>
       </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y10" s="6">
+        <f t="shared" si="0"/>
+        <v>2.11</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>560</v>
+      </c>
+      <c r="AA10" s="9">
+        <v>1183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>134</v>
+      <c r="C11" s="21">
+        <v>3</v>
       </c>
       <c r="D11" s="8">
         <v>2.33</v>
@@ -2067,10 +2165,10 @@
       <c r="S11" s="8">
         <v>2.3199999999999998</v>
       </c>
-      <c r="T11" s="24">
+      <c r="T11" s="25">
         <v>585</v>
       </c>
-      <c r="U11" s="25">
+      <c r="U11" s="26">
         <v>1359</v>
       </c>
       <c r="V11" s="8">
@@ -2082,16 +2180,26 @@
       <c r="X11" s="9">
         <v>1564</v>
       </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y11" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>585</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="20" t="s">
-        <v>134</v>
+      <c r="C12" s="21">
+        <v>3</v>
       </c>
       <c r="D12" s="8">
         <v>1.56</v>
@@ -2141,10 +2249,10 @@
       <c r="S12" s="8">
         <v>0.52</v>
       </c>
-      <c r="T12" s="24">
+      <c r="T12" s="25">
         <v>360</v>
       </c>
-      <c r="U12" s="25">
+      <c r="U12" s="26">
         <v>188</v>
       </c>
       <c r="V12" s="8">
@@ -2156,16 +2264,26 @@
       <c r="X12" s="9">
         <v>173</v>
       </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>450</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="20" t="s">
-        <v>134</v>
+      <c r="C13" s="21">
+        <v>3</v>
       </c>
       <c r="D13" s="8">
         <v>1.59</v>
@@ -2215,10 +2333,10 @@
       <c r="S13" s="8">
         <v>1.04</v>
       </c>
-      <c r="T13" s="24">
+      <c r="T13" s="25">
         <v>1215</v>
       </c>
-      <c r="U13" s="25">
+      <c r="U13" s="26">
         <v>1267</v>
       </c>
       <c r="V13" s="8">
@@ -2230,16 +2348,26 @@
       <c r="X13" s="9">
         <v>1557</v>
       </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y13" s="6">
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>1200</v>
+      </c>
+      <c r="AA13" s="9">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="35" t="s">
+      <c r="B14" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>134</v>
+      <c r="C14" s="21">
+        <v>3</v>
       </c>
       <c r="D14" s="8">
         <v>1.25</v>
@@ -2289,10 +2417,10 @@
       <c r="S14" s="8">
         <v>0.56000000000000005</v>
       </c>
-      <c r="T14" s="24">
+      <c r="T14" s="25">
         <v>585</v>
       </c>
-      <c r="U14" s="25">
+      <c r="U14" s="26">
         <v>327</v>
       </c>
       <c r="V14" s="8">
@@ -2304,16 +2432,26 @@
       <c r="X14" s="9">
         <v>320</v>
       </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y14" s="6">
+        <f t="shared" si="0"/>
+        <v>0.59</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA14" s="9">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="20" t="s">
-        <v>135</v>
+      <c r="C15" s="21">
+        <v>4</v>
       </c>
       <c r="D15" s="6">
         <v>1.39</v>
@@ -2363,10 +2501,10 @@
       <c r="S15" s="8">
         <v>0.83</v>
       </c>
-      <c r="T15" s="24">
+      <c r="T15" s="25">
         <v>585</v>
       </c>
-      <c r="U15" s="25">
+      <c r="U15" s="26">
         <v>487</v>
       </c>
       <c r="V15" s="8">
@@ -2378,16 +2516,26 @@
       <c r="X15" s="9">
         <v>402</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y15" s="6">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>585</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="20" t="s">
-        <v>135</v>
+      <c r="C16" s="21">
+        <v>4</v>
       </c>
       <c r="D16" s="8">
         <v>1.4</v>
@@ -2437,10 +2585,10 @@
       <c r="S16" s="8">
         <v>1.22</v>
       </c>
-      <c r="T16" s="24">
+      <c r="T16" s="25">
         <v>585</v>
       </c>
-      <c r="U16" s="25">
+      <c r="U16" s="26">
         <v>716</v>
       </c>
       <c r="V16" s="8">
@@ -2452,16 +2600,26 @@
       <c r="X16" s="9">
         <v>689</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y16" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>765</v>
+      </c>
+      <c r="AA16" s="9">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="20" t="s">
-        <v>136</v>
+      <c r="C17" s="21">
+        <v>5</v>
       </c>
       <c r="D17" s="8">
         <v>2.86</v>
@@ -2511,10 +2669,10 @@
       <c r="S17" s="8">
         <v>2.25</v>
       </c>
-      <c r="T17" s="24">
+      <c r="T17" s="25">
         <v>140</v>
       </c>
-      <c r="U17" s="25">
+      <c r="U17" s="26">
         <v>315</v>
       </c>
       <c r="V17" s="8">
@@ -2526,16 +2684,26 @@
       <c r="X17" s="9">
         <v>219</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.59</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>140</v>
+      </c>
+      <c r="AA17" s="9">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="20" t="s">
-        <v>136</v>
+      <c r="C18" s="21">
+        <v>5</v>
       </c>
       <c r="D18" s="8">
         <v>1.69</v>
@@ -2585,10 +2753,10 @@
       <c r="S18" s="8">
         <v>1.53</v>
       </c>
-      <c r="T18" s="24">
+      <c r="T18" s="25">
         <v>1035</v>
       </c>
-      <c r="U18" s="25">
+      <c r="U18" s="26">
         <v>1579</v>
       </c>
       <c r="V18" s="8">
@@ -2600,16 +2768,26 @@
       <c r="X18" s="9">
         <v>1437</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y18" s="6">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>1080</v>
+      </c>
+      <c r="AA18" s="9">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="20" t="s">
-        <v>136</v>
+      <c r="C19" s="21">
+        <v>5</v>
       </c>
       <c r="D19" s="8">
         <v>2.37</v>
@@ -2659,10 +2837,10 @@
       <c r="S19" s="8">
         <v>2.79</v>
       </c>
-      <c r="T19" s="24">
+      <c r="T19" s="25">
         <v>190</v>
       </c>
-      <c r="U19" s="25">
+      <c r="U19" s="26">
         <v>530</v>
       </c>
       <c r="V19" s="8">
@@ -2674,16 +2852,26 @@
       <c r="X19" s="9">
         <v>520</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y19" s="6">
+        <f t="shared" si="0"/>
+        <v>1.63</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>350</v>
+      </c>
+      <c r="AA19" s="9">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="20" t="s">
-        <v>136</v>
+      <c r="C20" s="21">
+        <v>5</v>
       </c>
       <c r="D20" s="8">
         <v>1.57</v>
@@ -2733,10 +2921,10 @@
       <c r="S20" s="8">
         <v>1.68</v>
       </c>
-      <c r="T20" s="24">
+      <c r="T20" s="25">
         <v>720</v>
       </c>
-      <c r="U20" s="25">
+      <c r="U20" s="26">
         <v>1212</v>
       </c>
       <c r="V20" s="8">
@@ -2748,16 +2936,26 @@
       <c r="X20" s="9">
         <v>1259</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y20" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>720</v>
+      </c>
+      <c r="AA20" s="9">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>136</v>
+      <c r="C21" s="21">
+        <v>5</v>
       </c>
       <c r="D21" s="8">
         <v>1.05</v>
@@ -2807,10 +3005,10 @@
       <c r="S21" s="8">
         <v>0.65</v>
       </c>
-      <c r="T21" s="24">
+      <c r="T21" s="25">
         <v>315</v>
       </c>
-      <c r="U21" s="25">
+      <c r="U21" s="26">
         <v>206</v>
       </c>
       <c r="V21" s="8">
@@ -2822,16 +3020,26 @@
       <c r="X21" s="9">
         <v>176</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y21" s="6">
+        <f t="shared" si="0"/>
+        <v>0.62</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>360</v>
+      </c>
+      <c r="AA21" s="9">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>137</v>
+      <c r="C22" s="21">
+        <v>6</v>
       </c>
       <c r="D22" s="8">
         <v>2.6</v>
@@ -2881,10 +3089,10 @@
       <c r="S22" s="8">
         <v>2.5499999999999998</v>
       </c>
-      <c r="T22" s="24">
+      <c r="T22" s="25">
         <v>810</v>
       </c>
-      <c r="U22" s="25">
+      <c r="U22" s="26">
         <v>2065</v>
       </c>
       <c r="V22" s="8">
@@ -2896,16 +3104,26 @@
       <c r="X22" s="9">
         <v>1937</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y22" s="6">
+        <f t="shared" si="0"/>
+        <v>2.35</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>810</v>
+      </c>
+      <c r="AA22" s="9">
+        <v>1903</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C23" s="20" t="s">
-        <v>137</v>
+      <c r="C23" s="21">
+        <v>6</v>
       </c>
       <c r="D23" s="8">
         <v>2.31</v>
@@ -2955,10 +3173,10 @@
       <c r="S23" s="8">
         <v>1.5</v>
       </c>
-      <c r="T23" s="24">
+      <c r="T23" s="25">
         <v>615</v>
       </c>
-      <c r="U23" s="25">
+      <c r="U23" s="26">
         <v>1014</v>
       </c>
       <c r="V23" s="8">
@@ -2970,16 +3188,26 @@
       <c r="X23" s="9">
         <v>1069</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y23" s="6">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA23" s="9">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="20" t="s">
-        <v>137</v>
+      <c r="C24" s="21">
+        <v>6</v>
       </c>
       <c r="D24" s="8">
         <v>1.39</v>
@@ -3029,10 +3257,10 @@
       <c r="S24" s="8">
         <v>1.1499999999999999</v>
       </c>
-      <c r="T24" s="24">
+      <c r="T24" s="25">
         <v>720</v>
       </c>
-      <c r="U24" s="25">
+      <c r="U24" s="26">
         <v>825</v>
       </c>
       <c r="V24" s="8">
@@ -3044,16 +3272,26 @@
       <c r="X24" s="9">
         <v>783</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y24" s="6">
+        <f t="shared" si="0"/>
+        <v>1.37</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>720</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>137</v>
+      <c r="C25" s="21">
+        <v>6</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="4"/>
@@ -3091,10 +3329,10 @@
       <c r="S25" s="8">
         <v>1.17</v>
       </c>
-      <c r="T25" s="24">
-        <v>675</v>
-      </c>
-      <c r="U25" s="25">
+      <c r="T25" s="25">
+        <v>675</v>
+      </c>
+      <c r="U25" s="26">
         <v>788</v>
       </c>
       <c r="V25" s="8">
@@ -3106,16 +3344,26 @@
       <c r="X25" s="9">
         <v>887</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y25" s="6">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA25" s="9">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>138</v>
+      <c r="C26" s="21">
+        <v>7</v>
       </c>
       <c r="D26" s="8">
         <v>1.24</v>
@@ -3165,10 +3413,10 @@
       <c r="S26" s="8">
         <v>1.65</v>
       </c>
-      <c r="T26" s="24">
+      <c r="T26" s="25">
         <v>540</v>
       </c>
-      <c r="U26" s="25">
+      <c r="U26" s="26">
         <v>891</v>
       </c>
       <c r="V26" s="8">
@@ -3180,16 +3428,26 @@
       <c r="X26" s="9">
         <v>852</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y26" s="6">
+        <f t="shared" si="0"/>
+        <v>1.81</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>585</v>
+      </c>
+      <c r="AA26" s="9">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="20" t="s">
-        <v>138</v>
+      <c r="C27" s="21">
+        <v>7</v>
       </c>
       <c r="D27" s="8">
         <v>1.08</v>
@@ -3239,10 +3497,10 @@
       <c r="S27" s="8">
         <v>0.35</v>
       </c>
-      <c r="T27" s="24">
+      <c r="T27" s="25">
         <v>585</v>
       </c>
-      <c r="U27" s="25">
+      <c r="U27" s="26">
         <v>204</v>
       </c>
       <c r="V27" s="8">
@@ -3254,16 +3512,26 @@
       <c r="X27" s="9">
         <v>266</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y27" s="6">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+      <c r="Z27" s="3">
+        <v>630</v>
+      </c>
+      <c r="AA27" s="9">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="20" t="s">
-        <v>138</v>
+      <c r="C28" s="21">
+        <v>7</v>
       </c>
       <c r="D28" s="8">
         <v>1.95</v>
@@ -3313,10 +3581,10 @@
       <c r="S28" s="8">
         <v>2.1</v>
       </c>
-      <c r="T28" s="24">
+      <c r="T28" s="25">
         <v>630</v>
       </c>
-      <c r="U28" s="25">
+      <c r="U28" s="26">
         <v>1321</v>
       </c>
       <c r="V28" s="8">
@@ -3328,16 +3596,26 @@
       <c r="X28" s="9">
         <v>1357</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y28" s="6">
+        <f t="shared" si="0"/>
+        <v>2.1</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>630</v>
+      </c>
+      <c r="AA28" s="9">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>138</v>
+      <c r="C29" s="21">
+        <v>7</v>
       </c>
       <c r="D29" s="8">
         <v>1.0900000000000001</v>
@@ -3387,10 +3665,10 @@
       <c r="S29" s="8">
         <v>1.25</v>
       </c>
-      <c r="T29" s="24">
+      <c r="T29" s="25">
         <v>180</v>
       </c>
-      <c r="U29" s="25">
+      <c r="U29" s="26">
         <v>225</v>
       </c>
       <c r="V29" s="8">
@@ -3402,16 +3680,26 @@
       <c r="X29" s="9">
         <v>242</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y29" s="6">
+        <f t="shared" si="0"/>
+        <v>1.41</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>225</v>
+      </c>
+      <c r="AA29" s="9">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>139</v>
+      <c r="C30" s="21">
+        <v>8</v>
       </c>
       <c r="D30" s="8">
         <v>1.41</v>
@@ -3461,10 +3749,10 @@
       <c r="S30" s="8">
         <v>0.95</v>
       </c>
-      <c r="T30" s="24">
+      <c r="T30" s="25">
         <v>540</v>
       </c>
-      <c r="U30" s="25">
+      <c r="U30" s="26">
         <v>515</v>
       </c>
       <c r="V30" s="8">
@@ -3476,16 +3764,26 @@
       <c r="X30" s="9">
         <v>537</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y30" s="6">
+        <f t="shared" si="0"/>
+        <v>0.61</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA30" s="9">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>139</v>
+      <c r="C31" s="21">
+        <v>8</v>
       </c>
       <c r="D31" s="8">
         <v>1.1599999999999999</v>
@@ -3535,10 +3833,10 @@
       <c r="S31" s="8">
         <v>0.46</v>
       </c>
-      <c r="T31" s="24">
+      <c r="T31" s="25">
         <v>540</v>
       </c>
-      <c r="U31" s="25">
+      <c r="U31" s="26">
         <v>251</v>
       </c>
       <c r="V31" s="8">
@@ -3550,16 +3848,26 @@
       <c r="X31" s="9">
         <v>203</v>
       </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y31" s="6">
+        <f t="shared" si="0"/>
+        <v>0.38</v>
+      </c>
+      <c r="Z31" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA31" s="9">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="35" t="s">
+      <c r="B32" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="C32" s="20" t="s">
-        <v>139</v>
+      <c r="C32" s="21">
+        <v>8</v>
       </c>
       <c r="D32" s="8">
         <v>1.31</v>
@@ -3609,10 +3917,10 @@
       <c r="S32" s="8">
         <v>1.45</v>
       </c>
-      <c r="T32" s="24">
+      <c r="T32" s="25">
         <v>585</v>
       </c>
-      <c r="U32" s="25">
+      <c r="U32" s="26">
         <v>846</v>
       </c>
       <c r="V32" s="8">
@@ -3624,16 +3932,26 @@
       <c r="X32" s="9">
         <v>994</v>
       </c>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y32" s="6">
+        <f t="shared" si="0"/>
+        <v>1.68</v>
+      </c>
+      <c r="Z32" s="3">
+        <v>585</v>
+      </c>
+      <c r="AA32" s="9">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="20" t="s">
-        <v>139</v>
+      <c r="C33" s="21">
+        <v>8</v>
       </c>
       <c r="D33" s="8">
         <v>1.06</v>
@@ -3683,10 +4001,10 @@
       <c r="S33" s="8">
         <v>0.33</v>
       </c>
-      <c r="T33" s="24">
+      <c r="T33" s="25">
         <v>540</v>
       </c>
-      <c r="U33" s="25">
+      <c r="U33" s="26">
         <v>180</v>
       </c>
       <c r="V33" s="8">
@@ -3698,16 +4016,26 @@
       <c r="X33" s="9">
         <v>138</v>
       </c>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y33" s="6">
+        <f t="shared" si="0"/>
+        <v>0.17</v>
+      </c>
+      <c r="Z33" s="3">
+        <v>765</v>
+      </c>
+      <c r="AA33" s="9">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="35" t="s">
+      <c r="B34" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="20" t="s">
-        <v>139</v>
+      <c r="C34" s="21">
+        <v>8</v>
       </c>
       <c r="D34" s="8">
         <v>1.06</v>
@@ -3757,10 +4085,10 @@
       <c r="S34" s="8">
         <v>1.24</v>
       </c>
-      <c r="T34" s="24">
+      <c r="T34" s="25">
         <v>585</v>
       </c>
-      <c r="U34" s="25">
+      <c r="U34" s="26">
         <v>728</v>
       </c>
       <c r="V34" s="8">
@@ -3772,16 +4100,26 @@
       <c r="X34" s="9">
         <v>690</v>
       </c>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y34" s="6">
+        <f t="shared" si="0"/>
+        <v>1.45</v>
+      </c>
+      <c r="Z34" s="3">
+        <v>585</v>
+      </c>
+      <c r="AA34" s="9">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="20" t="s">
-        <v>139</v>
+      <c r="C35" s="21">
+        <v>8</v>
       </c>
       <c r="D35" s="8">
         <v>1.21</v>
@@ -3831,10 +4169,10 @@
       <c r="S35" s="8">
         <v>0.56999999999999995</v>
       </c>
-      <c r="T35" s="24">
+      <c r="T35" s="25">
         <v>405</v>
       </c>
-      <c r="U35" s="25">
+      <c r="U35" s="26">
         <v>229</v>
       </c>
       <c r="V35" s="8">
@@ -3846,16 +4184,26 @@
       <c r="X35" s="9">
         <v>184</v>
       </c>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y35" s="6">
+        <f t="shared" si="0"/>
+        <v>0.42</v>
+      </c>
+      <c r="Z35" s="3">
+        <v>635</v>
+      </c>
+      <c r="AA35" s="9">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C36" s="20" t="s">
-        <v>140</v>
+      <c r="C36" s="21">
+        <v>9</v>
       </c>
       <c r="D36" s="8">
         <v>1.18</v>
@@ -3905,10 +4253,10 @@
       <c r="S36" s="8">
         <v>1.31</v>
       </c>
-      <c r="T36" s="24">
-        <v>675</v>
-      </c>
-      <c r="U36" s="25">
+      <c r="T36" s="25">
+        <v>675</v>
+      </c>
+      <c r="U36" s="26">
         <v>885</v>
       </c>
       <c r="V36" s="8">
@@ -3920,16 +4268,26 @@
       <c r="X36" s="9">
         <v>820</v>
       </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y36" s="6">
+        <f t="shared" si="0"/>
+        <v>1.32</v>
+      </c>
+      <c r="Z36" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA36" s="9">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="20" t="s">
-        <v>140</v>
+      <c r="C37" s="21">
+        <v>9</v>
       </c>
       <c r="D37" s="8">
         <v>1.1599999999999999</v>
@@ -3979,10 +4337,10 @@
       <c r="S37" s="8">
         <v>1.37</v>
       </c>
-      <c r="T37" s="24">
+      <c r="T37" s="25">
         <v>495</v>
       </c>
-      <c r="U37" s="25">
+      <c r="U37" s="26">
         <v>677</v>
       </c>
       <c r="V37" s="8">
@@ -3994,16 +4352,26 @@
       <c r="X37" s="9">
         <v>649</v>
       </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y37" s="6">
+        <f t="shared" si="0"/>
+        <v>1.52</v>
+      </c>
+      <c r="Z37" s="3">
+        <v>540</v>
+      </c>
+      <c r="AA37" s="9">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="20" t="s">
-        <v>140</v>
+      <c r="C38" s="21">
+        <v>9</v>
       </c>
       <c r="D38" s="8">
         <v>1.07</v>
@@ -4053,10 +4421,10 @@
       <c r="S38" s="8">
         <v>0.77</v>
       </c>
-      <c r="T38" s="24">
+      <c r="T38" s="25">
         <v>450</v>
       </c>
-      <c r="U38" s="25">
+      <c r="U38" s="26">
         <v>345</v>
       </c>
       <c r="V38" s="8">
@@ -4068,16 +4436,26 @@
       <c r="X38" s="9">
         <v>324</v>
       </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y38" s="6">
+        <f t="shared" si="0"/>
+        <v>0.48</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>765</v>
+      </c>
+      <c r="AA38" s="9">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="20" t="s">
-        <v>140</v>
+      <c r="C39" s="21">
+        <v>9</v>
       </c>
       <c r="D39" s="8">
         <v>1.04</v>
@@ -4127,10 +4505,10 @@
       <c r="S39" s="8">
         <v>0.38</v>
       </c>
-      <c r="T39" s="24">
+      <c r="T39" s="25">
         <v>495</v>
       </c>
-      <c r="U39" s="25">
+      <c r="U39" s="26">
         <v>189</v>
       </c>
       <c r="V39" s="8">
@@ -4142,16 +4520,26 @@
       <c r="X39" s="9">
         <v>347</v>
       </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y39" s="6">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+      <c r="Z39" s="3">
+        <v>765</v>
+      </c>
+      <c r="AA39" s="9">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="35" t="s">
+      <c r="B40" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="20" t="s">
-        <v>140</v>
+      <c r="C40" s="21">
+        <v>9</v>
       </c>
       <c r="D40" s="18"/>
       <c r="E40" s="4"/>
@@ -4175,10 +4563,10 @@
       <c r="S40" s="8">
         <v>0.64</v>
       </c>
-      <c r="T40" s="24">
+      <c r="T40" s="25">
         <v>450</v>
       </c>
-      <c r="U40" s="25">
+      <c r="U40" s="26">
         <v>288</v>
       </c>
       <c r="V40" s="8">
@@ -4190,16 +4578,26 @@
       <c r="X40" s="9">
         <v>425</v>
       </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y40" s="6">
+        <f t="shared" si="0"/>
+        <v>1.21</v>
+      </c>
+      <c r="Z40" s="3">
+        <v>495</v>
+      </c>
+      <c r="AA40" s="9">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="35" t="s">
+      <c r="B41" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="20" t="s">
-        <v>141</v>
+      <c r="C41" s="21">
+        <v>10</v>
       </c>
       <c r="D41" s="8">
         <v>1.31</v>
@@ -4222,10 +4620,10 @@
       <c r="J41" s="8">
         <v>1.19</v>
       </c>
-      <c r="K41" s="24">
+      <c r="K41" s="25">
         <v>810</v>
       </c>
-      <c r="L41" s="25">
+      <c r="L41" s="26">
         <v>963</v>
       </c>
       <c r="M41" s="8">
@@ -4249,10 +4647,10 @@
       <c r="S41" s="8">
         <v>0.92</v>
       </c>
-      <c r="T41" s="24">
+      <c r="T41" s="25">
         <v>810</v>
       </c>
-      <c r="U41" s="25">
+      <c r="U41" s="26">
         <v>748</v>
       </c>
       <c r="V41" s="8">
@@ -4264,16 +4662,26 @@
       <c r="X41" s="9">
         <v>889</v>
       </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y41" s="6">
+        <f t="shared" si="0"/>
+        <v>1.29</v>
+      </c>
+      <c r="Z41" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA41" s="9">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="35" t="s">
+      <c r="B42" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="20" t="s">
-        <v>141</v>
+      <c r="C42" s="21">
+        <v>10</v>
       </c>
       <c r="D42" s="8">
         <v>1.69</v>
@@ -4323,10 +4731,10 @@
       <c r="S42" s="8">
         <v>1.48</v>
       </c>
-      <c r="T42" s="24">
+      <c r="T42" s="25">
         <v>510</v>
       </c>
-      <c r="U42" s="25">
+      <c r="U42" s="26">
         <v>754</v>
       </c>
       <c r="V42" s="8">
@@ -4338,16 +4746,26 @@
       <c r="X42" s="9">
         <v>832</v>
       </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y42" s="6">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+      <c r="Z42" s="3">
+        <v>595</v>
+      </c>
+      <c r="AA42" s="9">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="35" t="s">
+      <c r="B43" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="20" t="s">
-        <v>141</v>
+      <c r="C43" s="21">
+        <v>10</v>
       </c>
       <c r="D43" s="8">
         <v>1.33</v>
@@ -4397,10 +4815,10 @@
       <c r="S43" s="8">
         <v>0.68</v>
       </c>
-      <c r="T43" s="24">
-        <v>675</v>
-      </c>
-      <c r="U43" s="25">
+      <c r="T43" s="25">
+        <v>675</v>
+      </c>
+      <c r="U43" s="26">
         <v>456</v>
       </c>
       <c r="V43" s="8">
@@ -4412,16 +4830,26 @@
       <c r="X43" s="9">
         <v>401</v>
       </c>
-    </row>
-    <row r="44" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y43" s="6">
+        <f t="shared" si="0"/>
+        <v>0.71</v>
+      </c>
+      <c r="Z43" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA43" s="9">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="35" t="s">
+      <c r="B44" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C44" s="20" t="s">
-        <v>141</v>
+      <c r="C44" s="21">
+        <v>10</v>
       </c>
       <c r="D44" s="8">
         <v>2.0099999999999998</v>
@@ -4477,7 +4905,7 @@
       <c r="U44" s="3">
         <v>196</v>
       </c>
-      <c r="V44" s="26">
+      <c r="V44" s="27">
         <v>0.7</v>
       </c>
       <c r="W44" s="3">
@@ -4486,16 +4914,26 @@
       <c r="X44" s="9">
         <v>251</v>
       </c>
-    </row>
-    <row r="45" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y44" s="6">
+        <f t="shared" si="0"/>
+        <v>0.53</v>
+      </c>
+      <c r="Z44" s="3">
+        <v>460</v>
+      </c>
+      <c r="AA44" s="9">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="20" t="s">
-        <v>141</v>
+      <c r="C45" s="21">
+        <v>10</v>
       </c>
       <c r="D45" s="8">
         <v>1.49</v>
@@ -4551,7 +4989,7 @@
       <c r="U45" s="3">
         <v>133</v>
       </c>
-      <c r="V45" s="26">
+      <c r="V45" s="27">
         <v>0.59</v>
       </c>
       <c r="W45" s="3">
@@ -4560,16 +4998,26 @@
       <c r="X45" s="9">
         <v>132</v>
       </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y45" s="6">
+        <f t="shared" si="0"/>
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="Z45" s="3">
+        <v>270</v>
+      </c>
+      <c r="AA45" s="9">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="35" t="s">
+      <c r="B46" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="C46" s="20" t="s">
-        <v>142</v>
+      <c r="C46" s="21">
+        <v>11</v>
       </c>
       <c r="D46" s="8">
         <v>1.56</v>
@@ -4625,7 +5073,7 @@
       <c r="U46" s="3">
         <v>569</v>
       </c>
-      <c r="V46" s="26">
+      <c r="V46" s="27">
         <v>1.4</v>
       </c>
       <c r="W46" s="3">
@@ -4634,16 +5082,26 @@
       <c r="X46" s="9">
         <v>587</v>
       </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y46" s="6">
+        <f t="shared" si="0"/>
+        <v>1.41</v>
+      </c>
+      <c r="Z46" s="3">
+        <v>490</v>
+      </c>
+      <c r="AA46" s="9">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="35" t="s">
+      <c r="B47" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C47" s="20" t="s">
-        <v>142</v>
+      <c r="C47" s="21">
+        <v>11</v>
       </c>
       <c r="D47" s="8">
         <v>1.49</v>
@@ -4699,7 +5157,7 @@
       <c r="U47" s="3">
         <v>746</v>
       </c>
-      <c r="V47" s="26">
+      <c r="V47" s="27">
         <v>0.99</v>
       </c>
       <c r="W47" s="3">
@@ -4708,16 +5166,26 @@
       <c r="X47" s="9">
         <v>801</v>
       </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y47" s="6">
+        <f t="shared" si="0"/>
+        <v>1.07</v>
+      </c>
+      <c r="Z47" s="3">
+        <v>810</v>
+      </c>
+      <c r="AA47" s="9">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="35" t="s">
+      <c r="B48" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="C48" s="20" t="s">
-        <v>142</v>
+      <c r="C48" s="21">
+        <v>11</v>
       </c>
       <c r="D48" s="8">
         <v>1.43</v>
@@ -4773,7 +5241,7 @@
       <c r="U48" s="3">
         <v>869</v>
       </c>
-      <c r="V48" s="26">
+      <c r="V48" s="27">
         <v>1.01</v>
       </c>
       <c r="W48" s="3">
@@ -4782,16 +5250,26 @@
       <c r="X48" s="9">
         <v>771</v>
       </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y48" s="6">
+        <f t="shared" si="0"/>
+        <v>1.35</v>
+      </c>
+      <c r="Z48" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA48" s="9">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="35" t="s">
+      <c r="B49" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="20" t="s">
-        <v>143</v>
+      <c r="C49" s="21">
+        <v>12</v>
       </c>
       <c r="D49" s="8">
         <v>1.7</v>
@@ -4847,7 +5325,7 @@
       <c r="U49" s="3">
         <v>1308</v>
       </c>
-      <c r="V49" s="26">
+      <c r="V49" s="27">
         <v>1.77</v>
       </c>
       <c r="W49" s="3">
@@ -4856,16 +5334,26 @@
       <c r="X49" s="9">
         <v>1197</v>
       </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y49" s="6">
+        <f t="shared" si="0"/>
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="Z49" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA49" s="9">
+        <v>1643</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="35" t="s">
+      <c r="B50" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C50" s="20" t="s">
-        <v>143</v>
+      <c r="C50" s="21">
+        <v>12</v>
       </c>
       <c r="D50" s="8">
         <v>1.6</v>
@@ -4921,7 +5409,7 @@
       <c r="U50" s="3">
         <v>1445</v>
       </c>
-      <c r="V50" s="26">
+      <c r="V50" s="27">
         <v>1.7</v>
       </c>
       <c r="W50" s="3">
@@ -4930,16 +5418,26 @@
       <c r="X50" s="9">
         <v>1373</v>
       </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y50" s="6">
+        <f t="shared" si="0"/>
+        <v>1.97</v>
+      </c>
+      <c r="Z50" s="3">
+        <v>810</v>
+      </c>
+      <c r="AA50" s="9">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="35" t="s">
+      <c r="B51" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="C51" s="20" t="s">
-        <v>143</v>
+      <c r="C51" s="21">
+        <v>12</v>
       </c>
       <c r="D51" s="8">
         <v>1.22</v>
@@ -4995,7 +5493,7 @@
       <c r="U51" s="3">
         <v>749</v>
       </c>
-      <c r="V51" s="26">
+      <c r="V51" s="27">
         <v>1.37</v>
       </c>
       <c r="W51" s="3">
@@ -5004,16 +5502,26 @@
       <c r="X51" s="9">
         <v>862</v>
       </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y51" s="6">
+        <f t="shared" si="0"/>
+        <v>1.63</v>
+      </c>
+      <c r="Z51" s="3">
+        <v>630</v>
+      </c>
+      <c r="AA51" s="9">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="35" t="s">
+      <c r="B52" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="C52" s="20" t="s">
-        <v>144</v>
+      <c r="C52" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="D52" s="8">
         <v>1.2</v>
@@ -5069,7 +5577,7 @@
       <c r="U52" s="3">
         <v>572</v>
       </c>
-      <c r="V52" s="26">
+      <c r="V52" s="27">
         <v>0.7</v>
       </c>
       <c r="W52" s="3">
@@ -5078,16 +5586,26 @@
       <c r="X52" s="9">
         <v>438</v>
       </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y52" s="6">
+        <f t="shared" si="0"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Z52" s="3">
+        <v>495</v>
+      </c>
+      <c r="AA52" s="9">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" s="35" t="s">
+      <c r="B53" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="C53" s="20" t="s">
-        <v>144</v>
+      <c r="C53" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="D53" s="8">
         <v>1.75</v>
@@ -5143,7 +5661,7 @@
       <c r="U53" s="3">
         <v>1050</v>
       </c>
-      <c r="V53" s="26">
+      <c r="V53" s="27">
         <v>1.21</v>
       </c>
       <c r="W53" s="3">
@@ -5152,16 +5670,26 @@
       <c r="X53" s="9">
         <v>1034</v>
       </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y53" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="Z53" s="3">
+        <v>820</v>
+      </c>
+      <c r="AA53" s="9">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
-      <c r="B54" s="35" t="s">
+      <c r="B54" s="33" t="s">
         <v>55</v>
       </c>
-      <c r="C54" s="20" t="s">
-        <v>144</v>
+      <c r="C54" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="D54" s="8">
         <v>2.4900000000000002</v>
@@ -5217,7 +5745,7 @@
       <c r="U54" s="3">
         <v>1859</v>
       </c>
-      <c r="V54" s="26">
+      <c r="V54" s="27">
         <v>3.13</v>
       </c>
       <c r="W54" s="3">
@@ -5226,16 +5754,26 @@
       <c r="X54" s="9">
         <v>1691</v>
       </c>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y54" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="Z54" s="3">
+        <v>685</v>
+      </c>
+      <c r="AA54" s="9">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
-      <c r="B55" s="35" t="s">
+      <c r="B55" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="C55" s="20" t="s">
-        <v>144</v>
+      <c r="C55" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="D55" s="8">
         <v>1.33</v>
@@ -5291,7 +5829,7 @@
       <c r="U55" s="3">
         <v>570</v>
       </c>
-      <c r="V55" s="26">
+      <c r="V55" s="27">
         <v>0.67</v>
       </c>
       <c r="W55" s="3">
@@ -5300,16 +5838,26 @@
       <c r="X55" s="9">
         <v>452</v>
       </c>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y55" s="6">
+        <f t="shared" si="0"/>
+        <v>0.78</v>
+      </c>
+      <c r="Z55" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA55" s="9">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
-      <c r="B56" s="35" t="s">
+      <c r="B56" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="20" t="s">
-        <v>144</v>
+      <c r="C56" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="D56" s="8">
         <v>1.02</v>
@@ -5365,7 +5913,7 @@
       <c r="U56" s="3">
         <v>501</v>
       </c>
-      <c r="V56" s="26">
+      <c r="V56" s="27">
         <v>0.95</v>
       </c>
       <c r="W56" s="3">
@@ -5374,16 +5922,26 @@
       <c r="X56" s="9">
         <v>642</v>
       </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y56" s="6">
+        <f t="shared" si="0"/>
+        <v>1.17</v>
+      </c>
+      <c r="Z56" s="3">
+        <v>720</v>
+      </c>
+      <c r="AA56" s="9">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
-      <c r="B57" s="35" t="s">
+      <c r="B57" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C57" s="20" t="s">
-        <v>144</v>
+      <c r="C57" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="D57" s="8">
         <v>1.84</v>
@@ -5439,7 +5997,7 @@
       <c r="U57" s="3">
         <v>1055</v>
       </c>
-      <c r="V57" s="26">
+      <c r="V57" s="27">
         <v>1.48</v>
       </c>
       <c r="W57" s="3">
@@ -5448,16 +6006,26 @@
       <c r="X57" s="9">
         <v>1195</v>
       </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y57" s="6">
+        <f t="shared" si="0"/>
+        <v>1.61</v>
+      </c>
+      <c r="Z57" s="3">
+        <v>810</v>
+      </c>
+      <c r="AA57" s="9">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="C58" s="20" t="s">
-        <v>119</v>
+      <c r="C58" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="D58" s="8">
         <v>1.45</v>
@@ -5513,7 +6081,7 @@
       <c r="U58" s="3">
         <v>687</v>
       </c>
-      <c r="V58" s="26">
+      <c r="V58" s="27">
         <v>0.94</v>
       </c>
       <c r="W58" s="3">
@@ -5522,16 +6090,26 @@
       <c r="X58" s="9">
         <v>592</v>
       </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y58" s="6">
+        <f t="shared" si="0"/>
+        <v>1.18</v>
+      </c>
+      <c r="Z58" s="3">
+        <v>585</v>
+      </c>
+      <c r="AA58" s="9">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
-      <c r="B59" s="35" t="s">
+      <c r="B59" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="C59" s="20" t="s">
-        <v>119</v>
+      <c r="C59" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="D59" s="8">
         <v>1.51</v>
@@ -5587,7 +6165,7 @@
       <c r="U59" s="3">
         <v>1053</v>
       </c>
-      <c r="V59" s="26">
+      <c r="V59" s="27">
         <v>1.78</v>
       </c>
       <c r="W59" s="3">
@@ -5596,16 +6174,26 @@
       <c r="X59" s="9">
         <v>1519</v>
       </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y59" s="6">
+        <f t="shared" si="0"/>
+        <v>1.64</v>
+      </c>
+      <c r="Z59" s="3">
+        <v>855</v>
+      </c>
+      <c r="AA59" s="9">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
-      <c r="B60" s="35" t="s">
+      <c r="B60" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="20" t="s">
-        <v>119</v>
+      <c r="C60" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="D60" s="8">
         <v>1.6</v>
@@ -5661,7 +6249,7 @@
       <c r="U60" s="3">
         <v>1574</v>
       </c>
-      <c r="V60" s="26">
+      <c r="V60" s="27">
         <v>1.57</v>
       </c>
       <c r="W60" s="3">
@@ -5670,16 +6258,26 @@
       <c r="X60" s="9">
         <v>1273</v>
       </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y60" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
+      <c r="Z60" s="3">
+        <v>830</v>
+      </c>
+      <c r="AA60" s="9">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
-      <c r="B61" s="35" t="s">
+      <c r="B61" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="C61" s="20" t="s">
-        <v>119</v>
+      <c r="C61" s="21" t="s">
+        <v>120</v>
       </c>
       <c r="D61" s="8">
         <v>1.04</v>
@@ -5735,7 +6333,7 @@
       <c r="U61" s="3">
         <v>1353</v>
       </c>
-      <c r="V61" s="26">
+      <c r="V61" s="27">
         <v>1.63</v>
       </c>
       <c r="W61" s="3">
@@ -5744,16 +6342,26 @@
       <c r="X61" s="9">
         <v>1393</v>
       </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y61" s="6">
+        <f t="shared" si="0"/>
+        <v>1.81</v>
+      </c>
+      <c r="Z61" s="3">
+        <v>900</v>
+      </c>
+      <c r="AA61" s="9">
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
-      <c r="B62" s="35" t="s">
+      <c r="B62" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="C62" s="20" t="s">
-        <v>120</v>
+      <c r="C62" s="21" t="s">
+        <v>121</v>
       </c>
       <c r="D62" s="8">
         <v>1.93</v>
@@ -5809,7 +6417,7 @@
       <c r="U62" s="3">
         <v>1596</v>
       </c>
-      <c r="V62" s="26">
+      <c r="V62" s="27">
         <v>2.2999999999999998</v>
       </c>
       <c r="W62" s="3">
@@ -5818,16 +6426,26 @@
       <c r="X62" s="9">
         <v>1655</v>
       </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y62" s="6">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="Z62" s="3">
+        <v>720</v>
+      </c>
+      <c r="AA62" s="9">
+        <v>1620</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
-      <c r="B63" s="35" t="s">
+      <c r="B63" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="C63" s="20" t="s">
-        <v>120</v>
+      <c r="C63" s="21" t="s">
+        <v>121</v>
       </c>
       <c r="D63" s="8">
         <v>1.1299999999999999</v>
@@ -5883,7 +6501,7 @@
       <c r="U63" s="3">
         <v>431</v>
       </c>
-      <c r="V63" s="26">
+      <c r="V63" s="27">
         <v>0.7</v>
       </c>
       <c r="W63" s="3">
@@ -5892,16 +6510,26 @@
       <c r="X63" s="9">
         <v>384</v>
       </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y63" s="6">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="Z63" s="3">
+        <v>630</v>
+      </c>
+      <c r="AA63" s="9">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
-      <c r="B64" s="35" t="s">
+      <c r="B64" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="C64" s="20" t="s">
-        <v>121</v>
+      <c r="C64" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="D64" s="8">
         <v>2.65</v>
@@ -5957,7 +6585,7 @@
       <c r="U64" s="3">
         <v>1600</v>
       </c>
-      <c r="V64" s="26">
+      <c r="V64" s="27">
         <v>3.3</v>
       </c>
       <c r="W64" s="3">
@@ -5966,16 +6594,26 @@
       <c r="X64" s="9">
         <v>1484</v>
       </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y64" s="6">
+        <f t="shared" si="0"/>
+        <v>2.99</v>
+      </c>
+      <c r="Z64" s="3">
+        <v>495</v>
+      </c>
+      <c r="AA64" s="9">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
-      <c r="B65" s="35" t="s">
+      <c r="B65" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C65" s="20" t="s">
-        <v>121</v>
+      <c r="C65" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="D65" s="8">
         <v>1.49</v>
@@ -6031,7 +6669,7 @@
       <c r="U65" s="3">
         <v>958</v>
       </c>
-      <c r="V65" s="26">
+      <c r="V65" s="27">
         <v>1.28</v>
       </c>
       <c r="W65" s="3">
@@ -6040,16 +6678,26 @@
       <c r="X65" s="9">
         <v>925</v>
       </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y65" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="Z65" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA65" s="9">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
-      <c r="B66" s="35" t="s">
+      <c r="B66" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="C66" s="20" t="s">
-        <v>121</v>
+      <c r="C66" s="21" t="s">
+        <v>122</v>
       </c>
       <c r="D66" s="8">
         <v>1.08</v>
@@ -6105,7 +6753,7 @@
       <c r="U66" s="3">
         <v>807</v>
       </c>
-      <c r="V66" s="26">
+      <c r="V66" s="27">
         <v>1.08</v>
       </c>
       <c r="W66" s="3">
@@ -6114,16 +6762,26 @@
       <c r="X66" s="9">
         <v>774</v>
       </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y66" s="6">
+        <f t="shared" si="0"/>
+        <v>1.34</v>
+      </c>
+      <c r="Z66" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA66" s="9">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
-      <c r="B67" s="35" t="s">
+      <c r="B67" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C67" s="20" t="s">
-        <v>122</v>
+      <c r="C67" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="D67" s="8">
         <v>2.2400000000000002</v>
@@ -6179,7 +6837,7 @@
       <c r="U67" s="3">
         <v>1941</v>
       </c>
-      <c r="V67" s="26">
+      <c r="V67" s="27">
         <v>2.4700000000000002</v>
       </c>
       <c r="W67" s="3">
@@ -6188,16 +6846,26 @@
       <c r="X67" s="9">
         <v>1667</v>
       </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y67" s="6">
+        <f t="shared" si="0"/>
+        <v>1.85</v>
+      </c>
+      <c r="Z67" s="3">
+        <v>810</v>
+      </c>
+      <c r="AA67" s="9">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
-      <c r="B68" s="35" t="s">
+      <c r="B68" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C68" s="20" t="s">
-        <v>122</v>
+      <c r="C68" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="D68" s="8">
         <v>1.88</v>
@@ -6253,7 +6921,7 @@
       <c r="U68" s="3">
         <v>1029</v>
       </c>
-      <c r="V68" s="26">
+      <c r="V68" s="27">
         <v>1.22</v>
       </c>
       <c r="W68" s="3">
@@ -6262,16 +6930,26 @@
       <c r="X68" s="9">
         <v>826</v>
       </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y68" s="6">
+        <f t="shared" ref="Y68:Y110" si="1">ROUND(AA68/Z68,2)</f>
+        <v>1.38</v>
+      </c>
+      <c r="Z68" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA68" s="9">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
-      <c r="B69" s="35" t="s">
+      <c r="B69" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C69" s="44" t="s">
-        <v>122</v>
+      <c r="C69" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="D69" s="8">
         <v>1.48</v>
@@ -6327,7 +7005,7 @@
       <c r="U69" s="3">
         <v>1444</v>
       </c>
-      <c r="V69" s="26">
+      <c r="V69" s="27">
         <v>1.68</v>
       </c>
       <c r="W69" s="3">
@@ -6336,16 +7014,26 @@
       <c r="X69" s="9">
         <v>1515</v>
       </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y69" s="6">
+        <f t="shared" si="1"/>
+        <v>1.97</v>
+      </c>
+      <c r="Z69" s="3">
+        <v>900</v>
+      </c>
+      <c r="AA69" s="9">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
-      <c r="B70" s="35" t="s">
+      <c r="B70" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="C70" s="20" t="s">
-        <v>122</v>
+      <c r="C70" s="21" t="s">
+        <v>123</v>
       </c>
       <c r="D70" s="18"/>
       <c r="E70" s="4"/>
@@ -6389,7 +7077,7 @@
       <c r="U70" s="3">
         <v>1159</v>
       </c>
-      <c r="V70" s="26">
+      <c r="V70" s="27">
         <v>1.95</v>
       </c>
       <c r="W70" s="3">
@@ -6398,16 +7086,26 @@
       <c r="X70" s="9">
         <v>1318</v>
       </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y70" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="Z70" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA70" s="9">
+        <v>1509</v>
+      </c>
+    </row>
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
-      <c r="B71" s="35" t="s">
+      <c r="B71" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C71" s="20" t="s">
-        <v>123</v>
+      <c r="C71" s="21" t="s">
+        <v>124</v>
       </c>
       <c r="D71" s="8">
         <v>3.35</v>
@@ -6463,7 +7161,7 @@
       <c r="U71" s="3">
         <v>1149</v>
       </c>
-      <c r="V71" s="26">
+      <c r="V71" s="27">
         <v>2.79</v>
       </c>
       <c r="W71" s="3">
@@ -6472,16 +7170,26 @@
       <c r="X71" s="9">
         <v>1383</v>
       </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y71" s="6">
+        <f t="shared" si="1"/>
+        <v>3.21</v>
+      </c>
+      <c r="Z71" s="3">
+        <v>415</v>
+      </c>
+      <c r="AA71" s="9">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
-      <c r="B72" s="35" t="s">
+      <c r="B72" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="20" t="s">
-        <v>123</v>
+      <c r="C72" s="21" t="s">
+        <v>124</v>
       </c>
       <c r="D72" s="8">
         <v>1.88</v>
@@ -6537,7 +7245,7 @@
       <c r="U72" s="3">
         <v>1536</v>
       </c>
-      <c r="V72" s="26">
+      <c r="V72" s="27">
         <v>2.2400000000000002</v>
       </c>
       <c r="W72" s="3">
@@ -6546,16 +7254,26 @@
       <c r="X72" s="9">
         <v>1613</v>
       </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y72" s="6">
+        <f t="shared" si="1"/>
+        <v>2.1</v>
+      </c>
+      <c r="Z72" s="3">
+        <v>775</v>
+      </c>
+      <c r="AA72" s="9">
+        <v>1626</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
-      <c r="B73" s="35" t="s">
+      <c r="B73" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="C73" s="20" t="s">
-        <v>123</v>
+      <c r="C73" s="21" t="s">
+        <v>124</v>
       </c>
       <c r="D73" s="8">
         <v>1.42</v>
@@ -6611,7 +7329,7 @@
       <c r="U73" s="3">
         <v>822</v>
       </c>
-      <c r="V73" s="26">
+      <c r="V73" s="27">
         <v>1.3</v>
       </c>
       <c r="W73" s="3">
@@ -6620,16 +7338,26 @@
       <c r="X73" s="9">
         <v>762</v>
       </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y73" s="6">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
+      <c r="Z73" s="3">
+        <v>630</v>
+      </c>
+      <c r="AA73" s="9">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="C74" s="20" t="s">
-        <v>123</v>
+      <c r="C74" s="21" t="s">
+        <v>124</v>
       </c>
       <c r="D74" s="8">
         <v>1.06</v>
@@ -6685,7 +7413,7 @@
       <c r="U74" s="3">
         <v>575</v>
       </c>
-      <c r="V74" s="26">
+      <c r="V74" s="27">
         <v>0.98</v>
       </c>
       <c r="W74" s="3">
@@ -6694,16 +7422,26 @@
       <c r="X74" s="9">
         <v>662</v>
       </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y74" s="6">
+        <f t="shared" si="1"/>
+        <v>1.24</v>
+      </c>
+      <c r="Z74" s="3">
+        <v>630</v>
+      </c>
+      <c r="AA74" s="9">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
-      <c r="B75" s="35" t="s">
+      <c r="B75" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="C75" s="20" t="s">
-        <v>123</v>
+      <c r="C75" s="21" t="s">
+        <v>124</v>
       </c>
       <c r="D75" s="8">
         <v>1.07</v>
@@ -6759,7 +7497,7 @@
       <c r="U75" s="3">
         <v>418</v>
       </c>
-      <c r="V75" s="26">
+      <c r="V75" s="27">
         <v>0.8</v>
       </c>
       <c r="W75" s="3">
@@ -6768,16 +7506,26 @@
       <c r="X75" s="9">
         <v>505</v>
       </c>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y75" s="6">
+        <f t="shared" si="1"/>
+        <v>0.74</v>
+      </c>
+      <c r="Z75" s="3">
+        <v>765</v>
+      </c>
+      <c r="AA75" s="9">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
-      <c r="B76" s="35" t="s">
+      <c r="B76" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="C76" s="20" t="s">
-        <v>123</v>
+      <c r="C76" s="21" t="s">
+        <v>124</v>
       </c>
       <c r="D76" s="18"/>
       <c r="E76" s="4"/>
@@ -6815,7 +7563,7 @@
       <c r="U76" s="3">
         <v>662</v>
       </c>
-      <c r="V76" s="26">
+      <c r="V76" s="27">
         <v>0.85</v>
       </c>
       <c r="W76" s="3">
@@ -6824,16 +7572,26 @@
       <c r="X76" s="9">
         <v>573</v>
       </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y76" s="6">
+        <f t="shared" si="1"/>
+        <v>0.87</v>
+      </c>
+      <c r="Z76" s="3">
+        <v>855</v>
+      </c>
+      <c r="AA76" s="9">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
-      <c r="B77" s="35" t="s">
+      <c r="B77" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="C77" s="20" t="s">
-        <v>123</v>
+      <c r="C77" s="21" t="s">
+        <v>124</v>
       </c>
       <c r="D77" s="18"/>
       <c r="E77" s="4"/>
@@ -6865,7 +7623,7 @@
       <c r="U77" s="3">
         <v>365</v>
       </c>
-      <c r="V77" s="26">
+      <c r="V77" s="27">
         <v>0.9</v>
       </c>
       <c r="W77" s="3">
@@ -6874,16 +7632,26 @@
       <c r="X77" s="9">
         <v>484</v>
       </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y77" s="6">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="Z77" s="3">
+        <v>810</v>
+      </c>
+      <c r="AA77" s="9">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
-      <c r="B78" s="35" t="s">
+      <c r="B78" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="C78" s="20" t="s">
-        <v>124</v>
+      <c r="C78" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="D78" s="8">
         <v>1.0900000000000001</v>
@@ -6939,7 +7707,7 @@
       <c r="U78" s="3">
         <v>670</v>
       </c>
-      <c r="V78" s="26">
+      <c r="V78" s="27">
         <v>1.04</v>
       </c>
       <c r="W78" s="3">
@@ -6948,16 +7716,26 @@
       <c r="X78" s="9">
         <v>702</v>
       </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y78" s="6">
+        <f t="shared" si="1"/>
+        <v>0.88</v>
+      </c>
+      <c r="Z78" s="3">
+        <v>900</v>
+      </c>
+      <c r="AA78" s="9">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
-      <c r="B79" s="35" t="s">
+      <c r="B79" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="C79" s="20" t="s">
-        <v>124</v>
+      <c r="C79" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="D79" s="8">
         <v>1.31</v>
@@ -7013,7 +7791,7 @@
       <c r="U79" s="3">
         <v>671</v>
       </c>
-      <c r="V79" s="26">
+      <c r="V79" s="27">
         <v>1.03</v>
       </c>
       <c r="W79" s="3">
@@ -7022,16 +7800,26 @@
       <c r="X79" s="9">
         <v>696</v>
       </c>
-    </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y79" s="6">
+        <f t="shared" si="1"/>
+        <v>0.94</v>
+      </c>
+      <c r="Z79" s="3">
+        <v>765</v>
+      </c>
+      <c r="AA79" s="9">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
-      <c r="B80" s="35" t="s">
+      <c r="B80" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="C80" s="20" t="s">
-        <v>124</v>
+      <c r="C80" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="D80" s="8">
         <v>1.01</v>
@@ -7087,7 +7875,7 @@
       <c r="U80" s="3">
         <v>345</v>
       </c>
-      <c r="V80" s="26">
+      <c r="V80" s="27">
         <v>0.62</v>
       </c>
       <c r="W80" s="3">
@@ -7096,16 +7884,26 @@
       <c r="X80" s="9">
         <v>361</v>
       </c>
-    </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y80" s="6">
+        <f t="shared" si="1"/>
+        <v>0.54</v>
+      </c>
+      <c r="Z80" s="3">
+        <v>855</v>
+      </c>
+      <c r="AA80" s="9">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
-      <c r="B81" s="35" t="s">
+      <c r="B81" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C81" s="20" t="s">
-        <v>124</v>
+      <c r="C81" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="D81" s="18"/>
       <c r="E81" s="4"/>
@@ -7143,7 +7941,7 @@
       <c r="U81" s="3">
         <v>168</v>
       </c>
-      <c r="V81" s="26">
+      <c r="V81" s="27">
         <v>0.38</v>
       </c>
       <c r="W81" s="3">
@@ -7152,16 +7950,26 @@
       <c r="X81" s="9">
         <v>188</v>
       </c>
-    </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y81" s="6">
+        <f t="shared" si="1"/>
+        <v>0.22</v>
+      </c>
+      <c r="Z81" s="3">
+        <v>750</v>
+      </c>
+      <c r="AA81" s="9">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
-      <c r="B82" s="35" t="s">
+      <c r="B82" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C82" s="20" t="s">
-        <v>124</v>
+      <c r="C82" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="D82" s="8">
         <v>1.18</v>
@@ -7217,7 +8025,7 @@
       <c r="U82" s="3">
         <v>805</v>
       </c>
-      <c r="V82" s="26">
+      <c r="V82" s="27">
         <v>1.23</v>
       </c>
       <c r="W82" s="3">
@@ -7226,16 +8034,26 @@
       <c r="X82" s="9">
         <v>832</v>
       </c>
-    </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y82" s="6">
+        <f t="shared" si="1"/>
+        <v>1.22</v>
+      </c>
+      <c r="Z82" s="3">
+        <v>720</v>
+      </c>
+      <c r="AA82" s="9">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
-      <c r="B83" s="35" t="s">
+      <c r="B83" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="C83" s="20" t="s">
-        <v>124</v>
+      <c r="C83" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="D83" s="8">
         <v>1.03</v>
@@ -7258,10 +8076,10 @@
       <c r="J83" s="8">
         <v>0.83</v>
       </c>
-      <c r="K83" s="28">
+      <c r="K83" s="29">
         <v>495</v>
       </c>
-      <c r="L83" s="30">
+      <c r="L83" s="31">
         <v>412</v>
       </c>
       <c r="M83" s="8">
@@ -7291,7 +8109,7 @@
       <c r="U83" s="3">
         <v>420</v>
       </c>
-      <c r="V83" s="26">
+      <c r="V83" s="27">
         <v>0.65</v>
       </c>
       <c r="W83" s="3">
@@ -7300,16 +8118,26 @@
       <c r="X83" s="9">
         <v>383</v>
       </c>
-    </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y83" s="6">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="Z83" s="3">
+        <v>765</v>
+      </c>
+      <c r="AA83" s="9">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
-      <c r="B84" s="35" t="s">
+      <c r="B84" s="33" t="s">
         <v>82</v>
       </c>
-      <c r="C84" s="20" t="s">
-        <v>124</v>
+      <c r="C84" s="21" t="s">
+        <v>125</v>
       </c>
       <c r="D84" s="18"/>
       <c r="E84" s="4"/>
@@ -7318,8 +8146,8 @@
       <c r="H84" s="4"/>
       <c r="I84" s="19"/>
       <c r="J84" s="18"/>
-      <c r="K84" s="29"/>
-      <c r="L84" s="31"/>
+      <c r="K84" s="30"/>
+      <c r="L84" s="32"/>
       <c r="M84" s="18"/>
       <c r="N84" s="4"/>
       <c r="O84" s="19"/>
@@ -7341,7 +8169,7 @@
       <c r="U84" s="3">
         <v>163</v>
       </c>
-      <c r="V84" s="26">
+      <c r="V84" s="27">
         <v>0.28999999999999998</v>
       </c>
       <c r="W84" s="3">
@@ -7350,16 +8178,26 @@
       <c r="X84" s="9">
         <v>197</v>
       </c>
-    </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y84" s="6">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="Z84" s="3">
+        <v>1035</v>
+      </c>
+      <c r="AA84" s="9">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
-      <c r="B85" s="35" t="s">
+      <c r="B85" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="C85" s="20" t="s">
-        <v>125</v>
+      <c r="C85" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="D85" s="8">
         <v>1.79</v>
@@ -7415,7 +8253,7 @@
       <c r="U85" s="3">
         <v>284</v>
       </c>
-      <c r="V85" s="26">
+      <c r="V85" s="27">
         <v>0.91</v>
       </c>
       <c r="W85" s="3">
@@ -7424,16 +8262,26 @@
       <c r="X85" s="9">
         <v>256</v>
       </c>
-    </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y85" s="6">
+        <f t="shared" si="1"/>
+        <v>0.81</v>
+      </c>
+      <c r="Z85" s="3">
+        <v>360</v>
+      </c>
+      <c r="AA85" s="9">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
-      <c r="B86" s="35" t="s">
+      <c r="B86" s="33" t="s">
         <v>84</v>
       </c>
-      <c r="C86" s="20" t="s">
-        <v>125</v>
+      <c r="C86" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="D86" s="8">
         <v>1.31</v>
@@ -7489,7 +8337,7 @@
       <c r="U86" s="3">
         <v>301</v>
       </c>
-      <c r="V86" s="26">
+      <c r="V86" s="27">
         <v>0.95</v>
       </c>
       <c r="W86" s="3">
@@ -7498,16 +8346,26 @@
       <c r="X86" s="9">
         <v>303</v>
       </c>
-    </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y86" s="6">
+        <f t="shared" si="1"/>
+        <v>0.78</v>
+      </c>
+      <c r="Z86" s="3">
+        <v>405</v>
+      </c>
+      <c r="AA86" s="9">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
-      <c r="B87" s="35" t="s">
+      <c r="B87" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="C87" s="20" t="s">
-        <v>125</v>
+      <c r="C87" s="21" t="s">
+        <v>126</v>
       </c>
       <c r="D87" s="8">
         <v>1.55</v>
@@ -7563,7 +8421,7 @@
       <c r="U87" s="3">
         <v>431</v>
       </c>
-      <c r="V87" s="26">
+      <c r="V87" s="27">
         <v>1.03</v>
       </c>
       <c r="W87" s="3">
@@ -7572,16 +8430,26 @@
       <c r="X87" s="9">
         <v>372</v>
       </c>
-    </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y87" s="6">
+        <f t="shared" si="1"/>
+        <v>0.79</v>
+      </c>
+      <c r="Z87" s="3">
+        <v>405</v>
+      </c>
+      <c r="AA87" s="9">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
-      <c r="B88" s="35" t="s">
+      <c r="B88" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="C88" s="20" t="s">
-        <v>126</v>
+      <c r="C88" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D88" s="18"/>
       <c r="E88" s="4"/>
@@ -7616,16 +8484,26 @@
       <c r="X88" s="9">
         <v>29</v>
       </c>
-    </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y88" s="6">
+        <f t="shared" si="1"/>
+        <v>0.59</v>
+      </c>
+      <c r="Z88" s="3">
+        <v>80</v>
+      </c>
+      <c r="AA88" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
-      <c r="B89" s="35" t="s">
+      <c r="B89" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="C89" s="20" t="s">
-        <v>126</v>
+      <c r="C89" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D89" s="8">
         <v>1.64</v>
@@ -7657,7 +8535,7 @@
       <c r="M89" s="8">
         <v>1.51</v>
       </c>
-      <c r="N89" s="24">
+      <c r="N89" s="25">
         <v>765</v>
       </c>
       <c r="O89" s="9">
@@ -7690,16 +8568,26 @@
       <c r="X89" s="9">
         <v>955</v>
       </c>
-    </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y89" s="6">
+        <f t="shared" si="1"/>
+        <v>1.51</v>
+      </c>
+      <c r="Z89" s="3">
+        <v>765</v>
+      </c>
+      <c r="AA89" s="9">
+        <v>1158</v>
+      </c>
+    </row>
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
-      <c r="B90" s="35" t="s">
+      <c r="B90" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="C90" s="20" t="s">
-        <v>126</v>
+      <c r="C90" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D90" s="8">
         <v>1.1499999999999999</v>
@@ -7764,16 +8652,26 @@
       <c r="X90" s="9">
         <v>634</v>
       </c>
-    </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y90" s="6">
+        <f t="shared" si="1"/>
+        <v>0.97</v>
+      </c>
+      <c r="Z90" s="3">
+        <v>675</v>
+      </c>
+      <c r="AA90" s="9">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
-      <c r="B91" s="35" t="s">
+      <c r="B91" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="C91" s="20" t="s">
-        <v>126</v>
+      <c r="C91" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D91" s="8">
         <v>1.02</v>
@@ -7838,16 +8736,26 @@
       <c r="X91" s="7">
         <v>537</v>
       </c>
-    </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y91" s="6">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+      <c r="Z91" s="2">
+        <v>720</v>
+      </c>
+      <c r="AA91" s="7">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
-      <c r="B92" s="35" t="s">
+      <c r="B92" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="20" t="s">
-        <v>126</v>
+      <c r="C92" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D92" s="8">
         <v>1.52</v>
@@ -7912,16 +8820,26 @@
       <c r="X92" s="7">
         <v>1033</v>
       </c>
-    </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y92" s="6">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="Z92" s="2">
+        <v>765</v>
+      </c>
+      <c r="AA92" s="7">
+        <v>1074</v>
+      </c>
+    </row>
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
-      <c r="B93" s="35" t="s">
+      <c r="B93" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="C93" s="20" t="s">
-        <v>126</v>
+      <c r="C93" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D93" s="8">
         <v>1.36</v>
@@ -7986,16 +8904,26 @@
       <c r="X93" s="7">
         <v>258</v>
       </c>
-    </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y93" s="6">
+        <f t="shared" si="1"/>
+        <v>0.51</v>
+      </c>
+      <c r="Z93" s="2">
+        <v>540</v>
+      </c>
+      <c r="AA93" s="7">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
-      <c r="B94" s="35" t="s">
+      <c r="B94" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="C94" s="20" t="s">
-        <v>126</v>
+      <c r="C94" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D94" s="8">
         <v>1.01</v>
@@ -8060,16 +8988,26 @@
       <c r="X94" s="7">
         <v>688</v>
       </c>
-    </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y94" s="6">
+        <f t="shared" si="1"/>
+        <v>1.37</v>
+      </c>
+      <c r="Z94" s="2">
+        <v>540</v>
+      </c>
+      <c r="AA94" s="7">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
-      <c r="B95" s="35" t="s">
+      <c r="B95" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C95" s="20" t="s">
-        <v>126</v>
+      <c r="C95" s="21" t="s">
+        <v>127</v>
       </c>
       <c r="D95" s="8">
         <v>1.0900000000000001</v>
@@ -8134,16 +9072,26 @@
       <c r="X95" s="7">
         <v>859</v>
       </c>
-    </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y95" s="6">
+        <f t="shared" si="1"/>
+        <v>1.81</v>
+      </c>
+      <c r="Z95" s="2">
+        <v>585</v>
+      </c>
+      <c r="AA95" s="7">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
-      <c r="B96" s="35" t="s">
+      <c r="B96" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="C96" s="20" t="s">
-        <v>127</v>
+      <c r="C96" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D96" s="8">
         <v>2.6</v>
@@ -8208,16 +9156,26 @@
       <c r="X96" s="7">
         <v>948</v>
       </c>
-    </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y96" s="6">
+        <f t="shared" si="1"/>
+        <v>1.82</v>
+      </c>
+      <c r="Z96" s="2">
+        <v>595</v>
+      </c>
+      <c r="AA96" s="7">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
-      <c r="B97" s="35" t="s">
+      <c r="B97" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="C97" s="20" t="s">
-        <v>127</v>
+      <c r="C97" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D97" s="8">
         <v>2</v>
@@ -8282,16 +9240,26 @@
       <c r="X97" s="7">
         <v>1033</v>
       </c>
-    </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y97" s="6">
+        <f t="shared" si="1"/>
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="Z97" s="2">
+        <v>495</v>
+      </c>
+      <c r="AA97" s="7">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98" s="35" t="s">
+      <c r="B98" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="20" t="s">
-        <v>127</v>
+      <c r="C98" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D98" s="8">
         <v>1.26</v>
@@ -8356,16 +9324,26 @@
       <c r="X98" s="7">
         <v>1107</v>
       </c>
-    </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y98" s="6">
+        <f t="shared" si="1"/>
+        <v>1.72</v>
+      </c>
+      <c r="Z98" s="2">
+        <v>630</v>
+      </c>
+      <c r="AA98" s="7">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
-      <c r="B99" s="35" t="s">
+      <c r="B99" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="C99" s="20" t="s">
-        <v>127</v>
+      <c r="C99" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D99" s="8">
         <v>1.04</v>
@@ -8430,16 +9408,26 @@
       <c r="X99" s="7">
         <v>414</v>
       </c>
-    </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y99" s="6">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+      <c r="Z99" s="2">
+        <v>585</v>
+      </c>
+      <c r="AA99" s="7">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
-      <c r="B100" s="35" t="s">
+      <c r="B100" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="C100" s="20" t="s">
-        <v>127</v>
+      <c r="C100" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D100" s="8">
         <v>1.74</v>
@@ -8504,16 +9492,26 @@
       <c r="X100" s="7">
         <v>941</v>
       </c>
-    </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y100" s="6">
+        <f t="shared" si="1"/>
+        <v>2.19</v>
+      </c>
+      <c r="Z100" s="2">
+        <v>495</v>
+      </c>
+      <c r="AA100" s="7">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
-      <c r="B101" s="35" t="s">
+      <c r="B101" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="C101" s="20" t="s">
-        <v>127</v>
+      <c r="C101" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D101" s="8">
         <v>1.02</v>
@@ -8578,16 +9576,26 @@
       <c r="X101" s="7">
         <v>1109</v>
       </c>
-    </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y101" s="6">
+        <f t="shared" si="1"/>
+        <v>1.98</v>
+      </c>
+      <c r="Z101" s="2">
+        <v>630</v>
+      </c>
+      <c r="AA101" s="7">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
-      <c r="B102" s="35" t="s">
+      <c r="B102" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C102" s="20" t="s">
-        <v>127</v>
+      <c r="C102" s="21" t="s">
+        <v>128</v>
       </c>
       <c r="D102" s="18"/>
       <c r="E102" s="4"/>
@@ -8628,16 +9636,26 @@
       <c r="X102" s="7">
         <v>1130</v>
       </c>
-    </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y102" s="6">
+        <f t="shared" si="1"/>
+        <v>1.58</v>
+      </c>
+      <c r="Z102" s="2">
+        <v>765</v>
+      </c>
+      <c r="AA102" s="7">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
-      <c r="B103" s="35" t="s">
+      <c r="B103" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="C103" s="20" t="s">
-        <v>128</v>
+      <c r="C103" s="21" t="s">
+        <v>129</v>
       </c>
       <c r="D103" s="8">
         <v>1.2</v>
@@ -8672,7 +9690,7 @@
       <c r="N103" s="3">
         <v>405</v>
       </c>
-      <c r="O103" s="27">
+      <c r="O103" s="28">
         <v>368</v>
       </c>
       <c r="P103" s="8">
@@ -8702,16 +9720,26 @@
       <c r="X103" s="7">
         <v>386</v>
       </c>
-    </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y103" s="6">
+        <f t="shared" si="1"/>
+        <v>0.98</v>
+      </c>
+      <c r="Z103" s="2">
+        <v>360</v>
+      </c>
+      <c r="AA103" s="7">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
-      <c r="B104" s="35" t="s">
+      <c r="B104" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="C104" s="20" t="s">
-        <v>128</v>
+      <c r="C104" s="21" t="s">
+        <v>129</v>
       </c>
       <c r="D104" s="8">
         <v>1.03</v>
@@ -8776,16 +9804,26 @@
       <c r="X104" s="7">
         <v>289</v>
       </c>
-    </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y104" s="6">
+        <f t="shared" si="1"/>
+        <v>0.54</v>
+      </c>
+      <c r="Z104" s="2">
+        <v>630</v>
+      </c>
+      <c r="AA104" s="7">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
-      <c r="B105" s="35" t="s">
+      <c r="B105" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C105" s="20" t="s">
-        <v>128</v>
+      <c r="C105" s="21" t="s">
+        <v>129</v>
       </c>
       <c r="D105" s="8">
         <v>1</v>
@@ -8850,16 +9888,26 @@
       <c r="X105" s="7">
         <v>330</v>
       </c>
-    </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y105" s="6">
+        <f t="shared" si="1"/>
+        <v>0.77</v>
+      </c>
+      <c r="Z105" s="2">
+        <v>585</v>
+      </c>
+      <c r="AA105" s="7">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
-      <c r="B106" s="35" t="s">
+      <c r="B106" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="C106" s="20" t="s">
-        <v>129</v>
+      <c r="C106" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="D106" s="8">
         <v>1.1499999999999999</v>
@@ -8924,16 +9972,26 @@
       <c r="X106" s="7">
         <v>914</v>
       </c>
-    </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y106" s="6">
+        <f t="shared" si="1"/>
+        <v>0.54</v>
+      </c>
+      <c r="Z106" s="2">
+        <v>855</v>
+      </c>
+      <c r="AA106" s="7">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
-      <c r="B107" s="35" t="s">
+      <c r="B107" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="C107" s="20" t="s">
-        <v>129</v>
+      <c r="C107" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="D107" s="8">
         <v>1.31</v>
@@ -8998,16 +10056,26 @@
       <c r="X107" s="7">
         <v>999</v>
       </c>
-    </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y107" s="6">
+        <f t="shared" si="1"/>
+        <v>1.94</v>
+      </c>
+      <c r="Z107" s="2">
+        <v>630</v>
+      </c>
+      <c r="AA107" s="7">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
-      <c r="B108" s="36" t="s">
+      <c r="B108" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C108" s="20" t="s">
-        <v>129</v>
+      <c r="C108" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="D108" s="6">
         <v>1.28</v>
@@ -9072,16 +10140,26 @@
       <c r="X108" s="7">
         <v>1220</v>
       </c>
-    </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y108" s="6">
+        <f t="shared" si="1"/>
+        <v>1.81</v>
+      </c>
+      <c r="Z108" s="2">
+        <v>720</v>
+      </c>
+      <c r="AA108" s="7">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
-      <c r="B109" s="36" t="s">
+      <c r="B109" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="C109" s="20" t="s">
-        <v>129</v>
+      <c r="C109" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="D109" s="6">
         <v>1.05</v>
@@ -9146,16 +10224,26 @@
       <c r="X109" s="7">
         <v>620</v>
       </c>
-    </row>
-    <row r="110" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y109" s="6">
+        <f t="shared" si="1"/>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Z109" s="2">
+        <v>720</v>
+      </c>
+      <c r="AA109" s="7">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="110" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
-      <c r="B110" s="36" t="s">
+      <c r="B110" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C110" s="20" t="s">
-        <v>129</v>
+      <c r="C110" s="21" t="s">
+        <v>130</v>
       </c>
       <c r="D110" s="10">
         <v>1.02</v>
@@ -9220,9 +10308,57 @@
       <c r="X110" s="12">
         <v>858</v>
       </c>
+      <c r="Y110" s="6">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="Z110" s="11">
+        <v>675</v>
+      </c>
+      <c r="AA110" s="12">
+        <v>946</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="P1:R1"/>
+    <mergeCell ref="S1:U1"/>
+  </mergeCells>
   <conditionalFormatting sqref="D3:D110 G3:G110 J3:J110 M3:M110 P3:P110 S3:S110 V3:V110">
+    <cfRule type="cellIs" dxfId="9" priority="8" operator="greaterThan">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="between">
+      <formula>2.01</formula>
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="10" operator="between">
+      <formula>1.01</formula>
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="between">
+      <formula>0.01</formula>
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="12" operator="between">
+      <formula>0.01</formula>
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D1:D1048576 G1:G1048576 J1:J1048576 M1:M1048576 P1:P1048576 S1:S1048576 V1:V1048576">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="between">
+      <formula>1.5</formula>
+      <formula>2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y110">
     <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>3</formula>
     </cfRule>
@@ -9243,7 +10379,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D1:D1048576 G1:G1048576 J1:J1048576 M1:M1048576 P1:P1048576 S1:S1048576 V1:V1048576">
+  <conditionalFormatting sqref="Y1:Y110">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>1.5</formula>
       <formula>2</formula>

</xml_diff>